<commit_message>
finished course details section
</commit_message>
<xml_diff>
--- a/static/data_base.xlsx
+++ b/static/data_base.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBEDD24-FC5A-40C4-AB61-417F6B27E4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FD1111-DC5D-4E59-A842-46335C7A7577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="105" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Country codes" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="573">
   <si>
     <t>ANDORRA</t>
   </si>
@@ -1733,6 +1733,15 @@
   </si>
   <si>
     <t>RQF8_RE</t>
+  </si>
+  <si>
+    <t>Course Level</t>
+  </si>
+  <si>
+    <t>RQF Level 4</t>
+  </si>
+  <si>
+    <t>RQF Level 7</t>
   </si>
 </sst>
 </file>
@@ -2177,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D253"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+    <sheetView topLeftCell="A210" workbookViewId="0">
+      <selection activeCell="I219" sqref="I219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4215,6 +4224,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4222,8 +4232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B266"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="B252" sqref="B252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6369,9 +6379,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C42813-83C0-4184-A8C5-3B5A0ED1D5C6}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -6380,9 +6390,10 @@
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>552</v>
       </c>
@@ -6392,8 +6403,11 @@
       <c r="C1" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>555</v>
       </c>
@@ -6403,8 +6417,11 @@
       <c r="C2" s="12">
         <v>45773</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>556</v>
       </c>
@@ -6414,8 +6431,11 @@
       <c r="C3" s="12">
         <v>46031</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>557</v>
       </c>
@@ -6424,6 +6444,9 @@
       </c>
       <c r="C4" s="12">
         <v>46503</v>
+      </c>
+      <c r="D4" t="s">
+        <v>571</v>
       </c>
     </row>
   </sheetData>
@@ -6435,14 +6458,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C290FFF-E80F-498E-B1C0-F26085EF6128}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>